<commit_message>
back memento and adapter debug
</commit_message>
<xml_diff>
--- a/src/solvers/School_timetabling_main/Solution/Solucao_por_dia_slot.xlsx
+++ b/src/solvers/School_timetabling_main/Solution/Solucao_por_dia_slot.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -558,12 +558,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Fernanda Dias</t>
+          <t>João Martins</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>BIOLOGIA</t>
+          <t>GEOGRAFIA</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -578,12 +578,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>João Martins</t>
+          <t>Gabriela Silva</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>GEOGRAFIA</t>
+          <t>FÍSICA</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -598,12 +598,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Gabriela Silva</t>
+          <t>Ricardo Fabião Amaro</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>FÍSICA</t>
+          <t>BIOLOGIA</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -618,12 +618,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Marcos Pereira</t>
+          <t>Ricardo Oliveira</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>BIOLOGIA</t>
+          <t>QUÍMICA</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -638,12 +638,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Ricardo Oliveira</t>
+          <t>Ricardo Fabião Amaro</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>QUÍMICA</t>
+          <t>BIOLOGIA</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -658,12 +658,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Ana Souza</t>
+          <t>Carlos Lima</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>MATEMÁTICA</t>
+          <t>HISTÓRIA</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -678,12 +678,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Carlos Lima</t>
+          <t>Gabriela Silva</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>HISTÓRIA</t>
+          <t>FÍSICA</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -698,12 +698,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Gabriela Silva</t>
+          <t>Ricardo Oliveira</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>FÍSICA</t>
+          <t>QUÍMICA</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -718,12 +718,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Marcos Pereira</t>
+          <t>Manoel Amaro</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>QUÍMICA</t>
+          <t>MATEMÁTICA</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -738,12 +738,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Ana Souza</t>
+          <t>Carlos Lima</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>MATEMÁTICA</t>
+          <t>HISTÓRIA</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -758,12 +758,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Carlos Lima</t>
+          <t>Gabriela Silva</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>HISTÓRIA</t>
+          <t>FÍSICA</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -778,12 +778,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Fernanda Dias</t>
+          <t>Luciana Costa</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>BIOLOGIA</t>
+          <t>MATEMÁTICA</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -798,12 +798,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Gabriela Silva</t>
+          <t>Ricardo Fabião Amaro</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>FÍSICA</t>
+          <t>BIOLOGIA</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -818,12 +818,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Fernanda Dias</t>
+          <t>Manoel Amaro</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>BIOLOGIA</t>
+          <t>QUÍMICA</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -838,12 +838,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Marcos Pereira</t>
+          <t>Ricardo Fabião Amaro</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>QUÍMICA</t>
+          <t>BIOLOGIA</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -858,12 +858,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Ana Souza</t>
+          <t>João Martins</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>MATEMÁTICA</t>
+          <t>GEOGRAFIA</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -878,12 +878,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>João Martins</t>
+          <t>Gabriela Silva</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>GEOGRAFIA</t>
+          <t>FÍSICA</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -898,12 +898,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Gabriela Silva</t>
+          <t>Marcos Pereira</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>FÍSICA</t>
+          <t>QUÍMICA</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -918,12 +918,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Marcos Pereira</t>
+          <t>Luciana Costa</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>QUÍMICA</t>
+          <t>MATEMÁTICA</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -938,12 +938,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Fernanda Dias</t>
+          <t>João Martins</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>BIOLOGIA</t>
+          <t>GEOGRAFIA</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -958,12 +958,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>João Martins</t>
+          <t>Gabriela Silva</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>GEOGRAFIA</t>
+          <t>FÍSICA</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -978,12 +978,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Gabriela Silva</t>
+          <t>Luciana Costa</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>FÍSICA</t>
+          <t>MATEMÁTICA</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -998,12 +998,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Luciana Costa</t>
+          <t>Ricardo Fabião Amaro</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>MATEMÁTICA</t>
+          <t>BIOLOGIA</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1018,12 +1018,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Marcos Pereira</t>
+          <t>Ricardo Oliveira</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>BIOLOGIA</t>
+          <t>QUÍMICA</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1038,12 +1038,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Ricardo Oliveira</t>
+          <t>Ricardo Fabião Amaro</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>QUÍMICA</t>
+          <t>BIOLOGIA</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1058,12 +1058,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Ana Souza</t>
+          <t>Carlos Lima</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>MATEMÁTICA</t>
+          <t>HISTÓRIA</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1078,12 +1078,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Carlos Lima</t>
+          <t>Gabriela Silva</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>HISTÓRIA</t>
+          <t>FÍSICA</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1098,12 +1098,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Gabriela Silva</t>
+          <t>Luciana Costa</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>FÍSICA</t>
+          <t>MATEMÁTICA</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1178,12 +1178,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Fernanda Dias</t>
+          <t>Gabriela Silva</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>BIOLOGIA</t>
+          <t>FÍSICA</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1198,12 +1198,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Gabriela Silva</t>
+          <t>Ricardo Fabião Amaro</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>FÍSICA</t>
+          <t>BIOLOGIA</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1218,12 +1218,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Fernanda Dias</t>
+          <t>Marcos Pereira</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>BIOLOGIA</t>
+          <t>QUÍMICA</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1238,12 +1238,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Marcos Pereira</t>
+          <t>Ricardo Fabião Amaro</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>QUÍMICA</t>
+          <t>BIOLOGIA</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1343,7 +1343,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>FÍSICA</t>
+          <t>MATEMÁTICA</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1398,12 +1398,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Fernanda Dias</t>
+          <t>Ricardo Fabião Amaro</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>BIOLOGIA</t>
+          <t>FÍSICA</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1412,7 +1412,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50">
@@ -1432,6 +1432,26 @@
         </is>
       </c>
       <c r="D50" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Ricardo Fabião Amaro</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>BIOLOGIA</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Sexta</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
gurobi to python MIP
</commit_message>
<xml_diff>
--- a/src/solvers/School_timetabling_main/Solution/Solucao_por_dia_slot.xlsx
+++ b/src/solvers/School_timetabling_main/Solution/Solucao_por_dia_slot.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -592,18 +592,18 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Ricardo Galvão Amaro</t>
+          <t>Marcos Pereira</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BIOLOGIA</t>
+          <t>QUÍMICA</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -612,18 +612,18 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Ricardo Oliveira</t>
+          <t>Ana Souza</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>QUÍMICA</t>
+          <t>BIOLOGIA</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -632,18 +632,18 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Ricardo Galvão Amaro</t>
+          <t>João Martins</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>BIOLOGIA</t>
+          <t>GEOGRAFIA</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -652,103 +652,103 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Carlos Lima</t>
+          <t>Gabriela Silva</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>HISTÓRIA</t>
+          <t>FÍSICA</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Terça</t>
+          <t>Segunda</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Gabriela Silva</t>
+          <t>Manoel Amaro</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>FÍSICA</t>
+          <t>MATEMÁTICA</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Terça</t>
+          <t>Segunda</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Ricardo Oliveira</t>
+          <t>Ana Souza</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>QUÍMICA</t>
+          <t>BIOLOGIA</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Terça</t>
+          <t>Segunda</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Manoel Amaro</t>
+          <t>João Martins</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>MATEMÁTICA</t>
+          <t>GEOGRAFIA</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Terça</t>
+          <t>Segunda</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Carlos Lima</t>
+          <t>Gabriela Silva</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>HISTÓRIA</t>
+          <t>FÍSICA</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Terça</t>
+          <t>Segunda</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -758,17 +758,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Gabriela Silva</t>
+          <t>Manoel Amaro</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>FÍSICA</t>
+          <t>MATEMÁTICA</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Terça</t>
+          <t>Segunda</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -778,21 +778,21 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Luciana Costa</t>
+          <t>Ricardo Oliveira</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>MATEMÁTICA</t>
+          <t>QUÍMICA</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Terça</t>
+          <t>Segunda</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
@@ -808,27 +808,27 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Terça</t>
+          <t>Segunda</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Manoel Amaro</t>
+          <t>Fernanda Dias</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>QUÍMICA</t>
+          <t>BIOLOGIA</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Terça</t>
+          <t>Segunda</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -838,17 +838,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Ricardo Galvão Amaro</t>
+          <t>Ricardo Oliveira</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>BIOLOGIA</t>
+          <t>QUÍMICA</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Terça</t>
+          <t>Segunda</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -858,17 +858,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>João Martins</t>
+          <t>Ana Souza</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>GEOGRAFIA</t>
+          <t>MATEMÁTICA</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Quarta</t>
+          <t>Terça</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -878,17 +878,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Gabriela Silva</t>
+          <t>Carlos Lima</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>FÍSICA</t>
+          <t>HISTÓRIA</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Quarta</t>
+          <t>Terça</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -898,17 +898,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Marcos Pereira</t>
+          <t>Gabriela Silva</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>QUÍMICA</t>
+          <t>FÍSICA</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Quarta</t>
+          <t>Terça</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -918,17 +918,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Luciana Costa</t>
+          <t>Marcos Pereira</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>MATEMÁTICA</t>
+          <t>QUÍMICA</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Quarta</t>
+          <t>Terça</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -938,21 +938,21 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>João Martins</t>
+          <t>Ana Souza</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>GEOGRAFIA</t>
+          <t>MATEMÁTICA</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Quarta</t>
+          <t>Terça</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -968,77 +968,77 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Quarta</t>
+          <t>Terça</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Luciana Costa</t>
+          <t>Marcos Pereira</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>MATEMÁTICA</t>
+          <t>QUÍMICA</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Quarta</t>
+          <t>Terça</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Ricardo Galvão Amaro</t>
+          <t>Ricardo Oliveira</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>BIOLOGIA</t>
+          <t>HISTÓRIA</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Quarta</t>
+          <t>Terça</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Ricardo Oliveira</t>
+          <t>Carlos Lima</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>QUÍMICA</t>
+          <t>HISTÓRIA</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Quarta</t>
+          <t>Terça</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Ricardo Galvão Amaro</t>
+          <t>Fernanda Dias</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1048,71 +1048,71 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Quarta</t>
+          <t>Terça</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Carlos Lima</t>
+          <t>Gabriela Silva</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>HISTÓRIA</t>
+          <t>FÍSICA</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Quinta</t>
+          <t>Terça</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Gabriela Silva</t>
+          <t>Luciana Costa</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>FÍSICA</t>
+          <t>MATEMÁTICA</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Quinta</t>
+          <t>Terça</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Luciana Costa</t>
+          <t>Ana Souza</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>MATEMÁTICA</t>
+          <t>FÍSICA</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Quinta</t>
+          <t>Terça</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35">
@@ -1123,22 +1123,22 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>QUÍMICA</t>
+          <t>HISTÓRIA</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Quinta</t>
+          <t>Terça</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Ana Souza</t>
+          <t>Manoel Amaro</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1148,7 +1148,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Quinta</t>
+          <t>Terça</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1158,17 +1158,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Carlos Lima</t>
+          <t>Ricardo Galvão Amaro</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>HISTÓRIA</t>
+          <t>BIOLOGIA</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Quinta</t>
+          <t>Terça</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1178,21 +1178,21 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Gabriela Silva</t>
+          <t>Manoel Amaro</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>FÍSICA</t>
+          <t>QUÍMICA</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Quinta</t>
+          <t>Terça</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39">
@@ -1208,11 +1208,11 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Quinta</t>
+          <t>Terça</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40">
@@ -1228,7 +1228,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Quinta</t>
+          <t>Terça</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1248,7 +1248,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Quinta</t>
+          <t>Terça</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1258,17 +1258,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Ana Souza</t>
+          <t>João Martins</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>MATEMÁTICA</t>
+          <t>GEOGRAFIA</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Sexta</t>
+          <t>Quarta</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -1278,17 +1278,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>João Martins</t>
+          <t>Gabriela Silva</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>GEOGRAFIA</t>
+          <t>FÍSICA</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Sexta</t>
+          <t>Quarta</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1308,7 +1308,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Sexta</t>
+          <t>Quarta</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1323,12 +1323,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>FÍSICA</t>
+          <t>MATEMÁTICA</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Sexta</t>
+          <t>Quarta</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1348,57 +1348,57 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Sexta</t>
+          <t>Quarta</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Fernanda Dias</t>
+          <t>João Martins</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>BIOLOGIA</t>
+          <t>GEOGRAFIA</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Sexta</t>
+          <t>Quarta</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>João Martins</t>
+          <t>Marcos Pereira</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>GEOGRAFIA</t>
+          <t>QUÍMICA</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Sexta</t>
+          <t>Quarta</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Ricardo Galvão Amaro</t>
+          <t>Manoel Amaro</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1408,50 +1408,1050 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Sexta</t>
+          <t>Quarta</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Marcos Pereira</t>
+          <t>João Martins</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>QUÍMICA</t>
+          <t>GEOGRAFIA</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Sexta</t>
+          <t>Quarta</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
+          <t>Gabriela Silva</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>FÍSICA</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Quarta</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Luciana Costa</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>MATEMÁTICA</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Quarta</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
           <t>Ricardo Galvão Amaro</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="B53" t="inlineStr">
         <is>
           <t>BIOLOGIA</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Quarta</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>João Martins</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>GEOGRAFIA</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Quarta</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Luciana Costa</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>MATEMÁTICA</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Quarta</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Manoel Amaro</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>FÍSICA</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Quarta</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Ricardo Galvão Amaro</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>BIOLOGIA</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Quarta</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Ricardo Oliveira</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>QUÍMICA</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Quarta</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Ricardo Galvão Amaro</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>BIOLOGIA</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Quarta</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Fernanda Dias</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>BIOLOGIA</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Quarta</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Ricardo Oliveira</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>QUÍMICA</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Quarta</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Ana Souza</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>MATEMÁTICA</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Quinta</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Carlos Lima</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>HISTÓRIA</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Quinta</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Luciana Costa</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>FÍSICA</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Quinta</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Ricardo Oliveira</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>QUÍMICA</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Quinta</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Ana Souza</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>MATEMÁTICA</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Quinta</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Marcos Pereira</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>QUÍMICA</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Quinta</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Luciana Costa</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>FÍSICA</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Quinta</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Ricardo Oliveira</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>HISTÓRIA</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Quinta</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Ana Souza</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>MATEMÁTICA</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Quinta</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Carlos Lima</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>HISTÓRIA</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Quinta</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Gabriela Silva</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>FÍSICA</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Quinta</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Ricardo Galvão Amaro</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>BIOLOGIA</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Quinta</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Ana Souza</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>MATEMÁTICA</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Quinta</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Fernanda Dias</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>BIOLOGIA</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Quinta</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Ricardo Oliveira</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>HISTÓRIA</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Quinta</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Ricardo Galvão Amaro</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>FÍSICA</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Quinta</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Fernanda Dias</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>QUÍMICA</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Quinta</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Ricardo Galvão Amaro</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>BIOLOGIA</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Quinta</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Fernanda Dias</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>QUÍMICA</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Quinta</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Ricardo Galvão Amaro</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>BIOLOGIA</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Quinta</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Ana Souza</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>MATEMÁTICA</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
         <is>
           <t>Sexta</t>
         </is>
       </c>
-      <c r="D51" t="n">
+      <c r="D82" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>João Martins</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>GEOGRAFIA</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Sexta</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Marcos Pereira</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>QUÍMICA</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Sexta</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Luciana Costa</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>FÍSICA</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Sexta</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Ana Souza</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>MATEMÁTICA</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Sexta</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>João Martins</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>GEOGRAFIA</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Sexta</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Marcos Pereira</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>QUÍMICA</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Sexta</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Luciana Costa</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>FÍSICA</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Sexta</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Ana Souza</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>MATEMÁTICA</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Sexta</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Fernanda Dias</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>BIOLOGIA</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Sexta</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>João Martins</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>GEOGRAFIA</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Sexta</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Ricardo Galvão Amaro</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>FÍSICA</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Sexta</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Ana Souza</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>MATEMÁTICA</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Sexta</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Fernanda Dias</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>BIOLOGIA</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Sexta</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>João Martins</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>GEOGRAFIA</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Sexta</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Ricardo Galvão Amaro</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>FÍSICA</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Sexta</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Fernanda Dias</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>QUÍMICA</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Sexta</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Ricardo Galvão Amaro</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>BIOLOGIA</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Sexta</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Fernanda Dias</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>QUÍMICA</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Sexta</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Ricardo Galvão Amaro</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>BIOLOGIA</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Sexta</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>